<commit_message>
funciona bien las rutas de accion
</commit_message>
<xml_diff>
--- a/canalizador/canalizador referencia lucas.xlsx
+++ b/canalizador/canalizador referencia lucas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rstaffolani\Desktop\SALUD\canalizador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rstaffolani\Desktop\unificar-archivos-ocasa-CM\canalizador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EB5B46-2BDB-4D71-AB45-B03F7DF06571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1299F1-97AF-46B8-95FA-776CA87C1BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{10834303-3970-4B37-8D4B-3A98A40CD95A}"/>
   </bookViews>
@@ -8735,8 +8735,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:E3398"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A2132" workbookViewId="0">
+      <selection activeCell="A2143" sqref="A2143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8776,7 +8776,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -8793,7 +8793,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
@@ -8810,7 +8810,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>12</v>
@@ -8827,7 +8827,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
@@ -8844,7 +8844,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
@@ -8861,7 +8861,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>12</v>
@@ -8878,7 +8878,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>12</v>
@@ -8895,7 +8895,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>12</v>
@@ -8912,7 +8912,7 @@
         <v>11</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>12</v>
@@ -8929,7 +8929,7 @@
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>12</v>
@@ -8946,7 +8946,7 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>12</v>
@@ -8963,7 +8963,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>12</v>
@@ -8980,7 +8980,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
@@ -8997,7 +8997,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>12</v>
@@ -9014,7 +9014,7 @@
         <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>12</v>
@@ -9031,7 +9031,7 @@
         <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>12</v>
@@ -9048,7 +9048,7 @@
         <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>12</v>
@@ -9065,7 +9065,7 @@
         <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>12</v>
@@ -9082,7 +9082,7 @@
         <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>12</v>
@@ -9099,7 +9099,7 @@
         <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>12</v>
@@ -9116,7 +9116,7 @@
         <v>11</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>12</v>
@@ -9133,7 +9133,7 @@
         <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>12</v>
@@ -9150,7 +9150,7 @@
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>12</v>
@@ -9167,7 +9167,7 @@
         <v>11</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>12</v>
@@ -9184,7 +9184,7 @@
         <v>11</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>12</v>
@@ -9201,7 +9201,7 @@
         <v>11</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>12</v>
@@ -9218,7 +9218,7 @@
         <v>11</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>12</v>
@@ -9235,7 +9235,7 @@
         <v>11</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>12</v>
@@ -9252,7 +9252,7 @@
         <v>11</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>12</v>
@@ -9269,7 +9269,7 @@
         <v>11</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>12</v>
@@ -9286,7 +9286,7 @@
         <v>11</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>12</v>
@@ -9303,7 +9303,7 @@
         <v>11</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>12</v>
@@ -9320,7 +9320,7 @@
         <v>11</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>12</v>
@@ -9337,7 +9337,7 @@
         <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>12</v>
@@ -9354,7 +9354,7 @@
         <v>11</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>12</v>
@@ -9371,7 +9371,7 @@
         <v>11</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>12</v>
@@ -9388,7 +9388,7 @@
         <v>11</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>12</v>
@@ -9405,7 +9405,7 @@
         <v>11</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>12</v>
@@ -9422,7 +9422,7 @@
         <v>11</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>12</v>
@@ -9439,7 +9439,7 @@
         <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>12</v>
@@ -9456,7 +9456,7 @@
         <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>12</v>
@@ -9473,7 +9473,7 @@
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>12</v>
@@ -9490,7 +9490,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>12</v>
@@ -9507,7 +9507,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>12</v>
@@ -9524,7 +9524,7 @@
         <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>12</v>
@@ -9541,7 +9541,7 @@
         <v>11</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>12</v>
@@ -9558,7 +9558,7 @@
         <v>11</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>12</v>
@@ -9575,7 +9575,7 @@
         <v>11</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>12</v>
@@ -9592,7 +9592,7 @@
         <v>11</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>12</v>
@@ -9609,7 +9609,7 @@
         <v>11</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>12</v>
@@ -9626,7 +9626,7 @@
         <v>11</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>12</v>
@@ -9643,7 +9643,7 @@
         <v>11</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>12</v>
@@ -9660,7 +9660,7 @@
         <v>11</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>12</v>
@@ -9677,7 +9677,7 @@
         <v>11</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>12</v>
@@ -9694,7 +9694,7 @@
         <v>11</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>12</v>
@@ -9711,7 +9711,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>12</v>
@@ -9728,7 +9728,7 @@
         <v>11</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>12</v>
@@ -9745,7 +9745,7 @@
         <v>11</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>12</v>
@@ -9762,7 +9762,7 @@
         <v>11</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>12</v>
@@ -9779,7 +9779,7 @@
         <v>11</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>12</v>
@@ -9796,7 +9796,7 @@
         <v>11</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>12</v>
@@ -9813,7 +9813,7 @@
         <v>11</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>12</v>
@@ -9830,7 +9830,7 @@
         <v>11</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>12</v>
@@ -9847,7 +9847,7 @@
         <v>11</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>12</v>
@@ -9864,7 +9864,7 @@
         <v>11</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>12</v>
@@ -9881,7 +9881,7 @@
         <v>11</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>12</v>
@@ -9898,7 +9898,7 @@
         <v>11</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>12</v>
@@ -9915,7 +9915,7 @@
         <v>11</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>12</v>
@@ -9932,7 +9932,7 @@
         <v>11</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>12</v>
@@ -9949,7 +9949,7 @@
         <v>11</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>12</v>
@@ -9966,7 +9966,7 @@
         <v>11</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>12</v>
@@ -9983,7 +9983,7 @@
         <v>11</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>12</v>
@@ -10000,7 +10000,7 @@
         <v>11</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>12</v>
@@ -10017,7 +10017,7 @@
         <v>11</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>12</v>
@@ -10034,7 +10034,7 @@
         <v>11</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>12</v>
@@ -10051,7 +10051,7 @@
         <v>11</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>12</v>
@@ -10068,7 +10068,7 @@
         <v>11</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>12</v>
@@ -10085,7 +10085,7 @@
         <v>11</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>12</v>
@@ -10102,7 +10102,7 @@
         <v>11</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>12</v>
@@ -10119,7 +10119,7 @@
         <v>11</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>12</v>
@@ -10136,7 +10136,7 @@
         <v>11</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>12</v>
@@ -10153,7 +10153,7 @@
         <v>11</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>12</v>
@@ -10170,7 +10170,7 @@
         <v>11</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>12</v>
@@ -10187,7 +10187,7 @@
         <v>11</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>12</v>
@@ -10204,7 +10204,7 @@
         <v>11</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>12</v>
@@ -10221,7 +10221,7 @@
         <v>11</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>12</v>
@@ -10238,7 +10238,7 @@
         <v>11</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>12</v>
@@ -10255,7 +10255,7 @@
         <v>11</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>12</v>
@@ -10272,7 +10272,7 @@
         <v>11</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>12</v>
@@ -10289,7 +10289,7 @@
         <v>11</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>12</v>
@@ -10306,7 +10306,7 @@
         <v>11</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>12</v>
@@ -10323,7 +10323,7 @@
         <v>11</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>12</v>
@@ -10340,7 +10340,7 @@
         <v>11</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>12</v>
@@ -10357,7 +10357,7 @@
         <v>11</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>12</v>
@@ -10374,7 +10374,7 @@
         <v>11</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>12</v>
@@ -10391,7 +10391,7 @@
         <v>11</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>12</v>
@@ -10408,7 +10408,7 @@
         <v>11</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>12</v>
@@ -10425,7 +10425,7 @@
         <v>11</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>12</v>
@@ -10442,7 +10442,7 @@
         <v>11</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>12</v>
@@ -10459,7 +10459,7 @@
         <v>11</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>12</v>
@@ -10476,7 +10476,7 @@
         <v>11</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E102" s="1" t="s">
         <v>12</v>
@@ -10493,7 +10493,7 @@
         <v>11</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E103" s="1" t="s">
         <v>12</v>
@@ -10510,7 +10510,7 @@
         <v>11</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>12</v>
@@ -10527,7 +10527,7 @@
         <v>11</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E105" s="1" t="s">
         <v>12</v>
@@ -10544,7 +10544,7 @@
         <v>11</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E106" s="1" t="s">
         <v>12</v>
@@ -10561,7 +10561,7 @@
         <v>11</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E107" s="1" t="s">
         <v>12</v>
@@ -10578,7 +10578,7 @@
         <v>11</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E108" s="1" t="s">
         <v>12</v>
@@ -10595,7 +10595,7 @@
         <v>11</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>12</v>
@@ -10612,7 +10612,7 @@
         <v>11</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E110" s="1" t="e">
         <v>#N/A</v>
@@ -10629,7 +10629,7 @@
         <v>11</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E111" s="1" t="e">
         <v>#N/A</v>
@@ -10646,7 +10646,7 @@
         <v>11</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E112" s="1" t="s">
         <v>12</v>
@@ -10663,7 +10663,7 @@
         <v>11</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>12</v>
@@ -10680,7 +10680,7 @@
         <v>11</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>12</v>
@@ -10697,7 +10697,7 @@
         <v>11</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E115" s="1" t="s">
         <v>12</v>
@@ -10714,7 +10714,7 @@
         <v>11</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E116" s="1" t="s">
         <v>12</v>
@@ -10731,7 +10731,7 @@
         <v>11</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E117" s="1" t="s">
         <v>12</v>
@@ -10748,7 +10748,7 @@
         <v>11</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>12</v>
@@ -10765,7 +10765,7 @@
         <v>11</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>12</v>
@@ -10782,7 +10782,7 @@
         <v>11</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>12</v>
@@ -10799,7 +10799,7 @@
         <v>11</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E121" s="1" t="s">
         <v>12</v>
@@ -10816,7 +10816,7 @@
         <v>11</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>12</v>
@@ -10833,7 +10833,7 @@
         <v>11</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>12</v>
@@ -10850,7 +10850,7 @@
         <v>11</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E124" s="1" t="s">
         <v>12</v>
@@ -10867,7 +10867,7 @@
         <v>11</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E125" s="1" t="s">
         <v>12</v>
@@ -10884,7 +10884,7 @@
         <v>11</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E126" s="1" t="s">
         <v>12</v>
@@ -10901,7 +10901,7 @@
         <v>11</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E127" s="1" t="s">
         <v>12</v>
@@ -10918,7 +10918,7 @@
         <v>11</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E128" s="1" t="s">
         <v>12</v>
@@ -10935,7 +10935,7 @@
         <v>11</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>12</v>
@@ -10952,7 +10952,7 @@
         <v>11</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>12</v>
@@ -10969,7 +10969,7 @@
         <v>11</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>12</v>
@@ -10986,7 +10986,7 @@
         <v>11</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>12</v>
@@ -11003,7 +11003,7 @@
         <v>11</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E133" s="1" t="s">
         <v>12</v>
@@ -11020,7 +11020,7 @@
         <v>11</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E134" s="1" t="s">
         <v>12</v>
@@ -11037,7 +11037,7 @@
         <v>11</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E135" s="1" t="s">
         <v>12</v>
@@ -11054,7 +11054,7 @@
         <v>11</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E136" s="1" t="s">
         <v>12</v>
@@ -11071,7 +11071,7 @@
         <v>11</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E137" s="1" t="s">
         <v>12</v>
@@ -11088,7 +11088,7 @@
         <v>11</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>12</v>
@@ -11105,7 +11105,7 @@
         <v>11</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>12</v>
@@ -11122,7 +11122,7 @@
         <v>11</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E140" s="1" t="s">
         <v>12</v>
@@ -11139,7 +11139,7 @@
         <v>11</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E141" s="1" t="s">
         <v>12</v>
@@ -11156,7 +11156,7 @@
         <v>11</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>12</v>
@@ -11173,7 +11173,7 @@
         <v>11</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>12</v>
@@ -11190,7 +11190,7 @@
         <v>11</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E144" s="1" t="s">
         <v>12</v>
@@ -11207,7 +11207,7 @@
         <v>11</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>12</v>
@@ -11224,7 +11224,7 @@
         <v>11</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>12</v>
@@ -11241,7 +11241,7 @@
         <v>11</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>12</v>
@@ -11258,7 +11258,7 @@
         <v>11</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E148" s="1" t="s">
         <v>12</v>
@@ -11275,7 +11275,7 @@
         <v>11</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E149" s="1" t="s">
         <v>12</v>
@@ -11292,7 +11292,7 @@
         <v>11</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>12</v>
@@ -11309,7 +11309,7 @@
         <v>11</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>12</v>
@@ -11326,7 +11326,7 @@
         <v>11</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E152" s="1" t="s">
         <v>12</v>
@@ -11343,7 +11343,7 @@
         <v>11</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E153" s="1" t="s">
         <v>12</v>
@@ -11360,7 +11360,7 @@
         <v>11</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>12</v>
@@ -11377,7 +11377,7 @@
         <v>11</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E155" s="1" t="s">
         <v>12</v>
@@ -11394,7 +11394,7 @@
         <v>11</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>12</v>
@@ -11411,7 +11411,7 @@
         <v>11</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E157" s="1" t="s">
         <v>12</v>
@@ -11428,7 +11428,7 @@
         <v>11</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>12</v>
@@ -11445,7 +11445,7 @@
         <v>11</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>12</v>
@@ -11462,7 +11462,7 @@
         <v>11</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E160" s="1" t="s">
         <v>12</v>
@@ -11479,7 +11479,7 @@
         <v>11</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E161" s="1" t="s">
         <v>12</v>
@@ -11496,7 +11496,7 @@
         <v>11</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E162" s="1" t="s">
         <v>12</v>
@@ -11513,7 +11513,7 @@
         <v>11</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>12</v>
@@ -11530,7 +11530,7 @@
         <v>11</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E164" s="1" t="s">
         <v>12</v>
@@ -11547,7 +11547,7 @@
         <v>11</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E165" s="1" t="s">
         <v>12</v>
@@ -11564,7 +11564,7 @@
         <v>11</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E166" s="1" t="s">
         <v>12</v>
@@ -11581,7 +11581,7 @@
         <v>11</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>12</v>
@@ -11598,7 +11598,7 @@
         <v>11</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E168" s="1" t="s">
         <v>12</v>
@@ -11615,7 +11615,7 @@
         <v>11</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E169" s="1" t="s">
         <v>12</v>
@@ -11632,7 +11632,7 @@
         <v>11</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E170" s="1" t="s">
         <v>12</v>
@@ -11649,7 +11649,7 @@
         <v>11</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E171" s="1" t="s">
         <v>12</v>
@@ -11666,7 +11666,7 @@
         <v>11</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E172" s="1" t="s">
         <v>12</v>
@@ -11683,7 +11683,7 @@
         <v>11</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>12</v>
@@ -11700,7 +11700,7 @@
         <v>11</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E174" s="1" t="s">
         <v>12</v>
@@ -11717,7 +11717,7 @@
         <v>11</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E175" s="1" t="s">
         <v>12</v>
@@ -11734,7 +11734,7 @@
         <v>11</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>12</v>
@@ -11751,7 +11751,7 @@
         <v>11</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>12</v>
@@ -11768,7 +11768,7 @@
         <v>11</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>12</v>
@@ -11785,7 +11785,7 @@
         <v>11</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>12</v>
@@ -11802,7 +11802,7 @@
         <v>11</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>12</v>
@@ -11819,7 +11819,7 @@
         <v>11</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>12</v>
@@ -11836,7 +11836,7 @@
         <v>11</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>12</v>
@@ -11853,7 +11853,7 @@
         <v>11</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>12</v>
@@ -11870,7 +11870,7 @@
         <v>11</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>12</v>
@@ -11887,7 +11887,7 @@
         <v>11</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>12</v>
@@ -11904,7 +11904,7 @@
         <v>11</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>12</v>
@@ -11921,7 +11921,7 @@
         <v>11</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>12</v>
@@ -11938,7 +11938,7 @@
         <v>11</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>12</v>
@@ -11955,7 +11955,7 @@
         <v>11</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>12</v>
@@ -11972,7 +11972,7 @@
         <v>11</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>12</v>
@@ -11989,7 +11989,7 @@
         <v>11</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>12</v>
@@ -12006,7 +12006,7 @@
         <v>11</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>12</v>
@@ -12023,7 +12023,7 @@
         <v>11</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>12</v>
@@ -12040,7 +12040,7 @@
         <v>11</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>12</v>
@@ -12057,7 +12057,7 @@
         <v>11</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>12</v>
@@ -12074,7 +12074,7 @@
         <v>11</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>12</v>
@@ -12091,7 +12091,7 @@
         <v>11</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>12</v>
@@ -12108,7 +12108,7 @@
         <v>11</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>12</v>
@@ -12125,7 +12125,7 @@
         <v>11</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>12</v>
@@ -12142,7 +12142,7 @@
         <v>11</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>12</v>
@@ -12159,7 +12159,7 @@
         <v>11</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>12</v>
@@ -12176,7 +12176,7 @@
         <v>11</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>12</v>
@@ -12193,7 +12193,7 @@
         <v>11</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>12</v>
@@ -12210,7 +12210,7 @@
         <v>11</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>12</v>
@@ -12227,7 +12227,7 @@
         <v>11</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>12</v>
@@ -12244,7 +12244,7 @@
         <v>11</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E206" s="1" t="s">
         <v>12</v>
@@ -12261,7 +12261,7 @@
         <v>11</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E207" s="1" t="s">
         <v>12</v>
@@ -12278,7 +12278,7 @@
         <v>11</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E208" s="1" t="s">
         <v>12</v>
@@ -12295,7 +12295,7 @@
         <v>11</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E209" s="1" t="s">
         <v>12</v>
@@ -12312,7 +12312,7 @@
         <v>11</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E210" s="1" t="s">
         <v>12</v>
@@ -12329,7 +12329,7 @@
         <v>11</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E211" s="1" t="s">
         <v>12</v>
@@ -12346,7 +12346,7 @@
         <v>11</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>12</v>
@@ -12363,7 +12363,7 @@
         <v>11</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>12</v>
@@ -12380,7 +12380,7 @@
         <v>11</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>12</v>
@@ -12397,7 +12397,7 @@
         <v>11</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>12</v>
@@ -12414,7 +12414,7 @@
         <v>11</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>12</v>
@@ -12431,7 +12431,7 @@
         <v>11</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E217" s="1" t="s">
         <v>12</v>
@@ -12448,7 +12448,7 @@
         <v>11</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E218" s="1" t="s">
         <v>12</v>
@@ -12465,7 +12465,7 @@
         <v>11</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E219" s="1" t="s">
         <v>12</v>
@@ -12482,7 +12482,7 @@
         <v>11</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E220" s="1" t="s">
         <v>12</v>
@@ -12499,7 +12499,7 @@
         <v>11</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E221" s="1" t="s">
         <v>12</v>
@@ -12516,7 +12516,7 @@
         <v>11</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E222" s="1" t="s">
         <v>12</v>
@@ -12533,7 +12533,7 @@
         <v>11</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E223" s="1" t="s">
         <v>12</v>
@@ -12550,7 +12550,7 @@
         <v>11</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E224" s="1" t="s">
         <v>12</v>
@@ -12567,7 +12567,7 @@
         <v>11</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E225" s="1" t="s">
         <v>12</v>
@@ -12584,7 +12584,7 @@
         <v>11</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E226" s="1" t="s">
         <v>12</v>
@@ -12601,7 +12601,7 @@
         <v>11</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E227" s="1" t="s">
         <v>12</v>
@@ -12618,7 +12618,7 @@
         <v>11</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E228" s="1" t="s">
         <v>12</v>
@@ -12635,7 +12635,7 @@
         <v>11</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E229" s="1" t="s">
         <v>12</v>
@@ -12652,7 +12652,7 @@
         <v>11</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E230" s="1" t="s">
         <v>12</v>
@@ -12669,7 +12669,7 @@
         <v>11</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E231" s="1" t="s">
         <v>12</v>
@@ -12686,7 +12686,7 @@
         <v>11</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E232" s="1" t="s">
         <v>12</v>
@@ -12703,7 +12703,7 @@
         <v>11</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E233" s="1" t="s">
         <v>12</v>
@@ -12720,7 +12720,7 @@
         <v>11</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E234" s="1" t="s">
         <v>12</v>
@@ -12737,7 +12737,7 @@
         <v>11</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E235" s="1" t="s">
         <v>12</v>
@@ -12754,7 +12754,7 @@
         <v>11</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E236" s="1" t="s">
         <v>12</v>
@@ -12771,7 +12771,7 @@
         <v>11</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E237" s="1" t="s">
         <v>12</v>
@@ -12788,7 +12788,7 @@
         <v>11</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E238" s="1" t="s">
         <v>12</v>
@@ -12805,7 +12805,7 @@
         <v>11</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E239" s="1" t="s">
         <v>12</v>
@@ -12822,7 +12822,7 @@
         <v>11</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E240" s="1" t="s">
         <v>12</v>
@@ -12839,7 +12839,7 @@
         <v>11</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E241" s="1" t="s">
         <v>12</v>
@@ -12856,7 +12856,7 @@
         <v>11</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E242" s="1" t="s">
         <v>12</v>
@@ -12873,7 +12873,7 @@
         <v>11</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E243" s="1" t="s">
         <v>12</v>
@@ -12890,7 +12890,7 @@
         <v>11</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E244" s="1" t="s">
         <v>12</v>
@@ -12907,7 +12907,7 @@
         <v>11</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E245" s="1" t="s">
         <v>12</v>
@@ -12924,7 +12924,7 @@
         <v>11</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E246" s="1" t="s">
         <v>12</v>
@@ -12941,7 +12941,7 @@
         <v>11</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E247" s="1" t="s">
         <v>12</v>
@@ -12958,7 +12958,7 @@
         <v>11</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E248" s="1" t="s">
         <v>12</v>
@@ -12975,7 +12975,7 @@
         <v>11</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E249" s="1" t="s">
         <v>12</v>
@@ -12992,7 +12992,7 @@
         <v>11</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E250" s="1" t="s">
         <v>12</v>
@@ -13009,7 +13009,7 @@
         <v>11</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E251" s="1" t="s">
         <v>12</v>
@@ -13026,7 +13026,7 @@
         <v>11</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E252" s="1" t="s">
         <v>12</v>
@@ -13043,7 +13043,7 @@
         <v>11</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E253" s="1" t="s">
         <v>12</v>
@@ -13060,7 +13060,7 @@
         <v>11</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E254" s="1" t="s">
         <v>12</v>
@@ -13077,7 +13077,7 @@
         <v>11</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E255" s="1" t="s">
         <v>12</v>
@@ -13094,7 +13094,7 @@
         <v>11</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E256" s="1" t="s">
         <v>12</v>
@@ -13111,7 +13111,7 @@
         <v>11</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E257" s="1" t="s">
         <v>12</v>
@@ -13128,7 +13128,7 @@
         <v>11</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E258" s="1" t="s">
         <v>12</v>
@@ -13145,7 +13145,7 @@
         <v>11</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E259" s="1" t="s">
         <v>12</v>
@@ -13162,7 +13162,7 @@
         <v>11</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E260" s="1" t="s">
         <v>12</v>
@@ -13179,7 +13179,7 @@
         <v>11</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E261" s="1" t="s">
         <v>12</v>
@@ -13196,7 +13196,7 @@
         <v>11</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E262" s="1" t="s">
         <v>12</v>
@@ -13213,7 +13213,7 @@
         <v>11</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E263" s="1" t="s">
         <v>12</v>
@@ -13230,7 +13230,7 @@
         <v>11</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E264" s="1" t="s">
         <v>12</v>
@@ -13247,7 +13247,7 @@
         <v>11</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E265" s="1" t="s">
         <v>12</v>
@@ -13264,7 +13264,7 @@
         <v>11</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E266" s="1" t="s">
         <v>12</v>
@@ -13281,7 +13281,7 @@
         <v>11</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E267" s="1" t="s">
         <v>12</v>
@@ -13298,7 +13298,7 @@
         <v>11</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E268" s="1" t="s">
         <v>12</v>
@@ -13315,7 +13315,7 @@
         <v>11</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E269" s="1" t="s">
         <v>12</v>
@@ -13332,7 +13332,7 @@
         <v>11</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E270" s="1" t="s">
         <v>12</v>
@@ -13349,7 +13349,7 @@
         <v>11</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E271" s="1" t="s">
         <v>12</v>
@@ -13366,7 +13366,7 @@
         <v>11</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E272" s="1" t="s">
         <v>12</v>
@@ -13383,7 +13383,7 @@
         <v>11</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E273" s="1" t="s">
         <v>12</v>
@@ -13400,7 +13400,7 @@
         <v>11</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E274" s="1" t="s">
         <v>12</v>
@@ -13417,7 +13417,7 @@
         <v>11</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E275" s="1" t="s">
         <v>12</v>
@@ -13434,7 +13434,7 @@
         <v>11</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E276" s="1" t="s">
         <v>12</v>
@@ -13451,7 +13451,7 @@
         <v>11</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E277" s="1" t="s">
         <v>12</v>
@@ -13468,7 +13468,7 @@
         <v>11</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E278" s="1" t="s">
         <v>12</v>
@@ -13485,7 +13485,7 @@
         <v>11</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E279" s="1" t="s">
         <v>12</v>
@@ -13502,7 +13502,7 @@
         <v>11</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E280" s="1" t="s">
         <v>12</v>
@@ -13519,7 +13519,7 @@
         <v>11</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E281" s="1" t="s">
         <v>12</v>
@@ -13536,7 +13536,7 @@
         <v>11</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E282" s="1" t="s">
         <v>12</v>
@@ -13553,7 +13553,7 @@
         <v>11</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E283" s="1" t="s">
         <v>12</v>
@@ -13570,7 +13570,7 @@
         <v>11</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E284" s="1" t="s">
         <v>12</v>
@@ -13587,7 +13587,7 @@
         <v>11</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E285" s="1" t="s">
         <v>12</v>
@@ -13604,7 +13604,7 @@
         <v>11</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E286" s="1" t="s">
         <v>12</v>
@@ -13621,7 +13621,7 @@
         <v>11</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E287" s="1" t="s">
         <v>12</v>
@@ -13638,7 +13638,7 @@
         <v>11</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E288" s="1" t="s">
         <v>12</v>
@@ -13655,7 +13655,7 @@
         <v>11</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E289" s="1" t="s">
         <v>12</v>
@@ -13672,7 +13672,7 @@
         <v>11</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E290" s="1" t="s">
         <v>12</v>
@@ -13689,7 +13689,7 @@
         <v>11</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E291" s="1" t="s">
         <v>12</v>
@@ -13706,7 +13706,7 @@
         <v>11</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E292" s="1" t="s">
         <v>12</v>
@@ -13723,7 +13723,7 @@
         <v>11</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E293" s="1" t="s">
         <v>12</v>
@@ -13740,7 +13740,7 @@
         <v>11</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E294" s="1" t="s">
         <v>12</v>
@@ -13757,7 +13757,7 @@
         <v>11</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E295" s="1" t="s">
         <v>12</v>
@@ -13774,7 +13774,7 @@
         <v>11</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E296" s="1" t="s">
         <v>12</v>
@@ -13791,7 +13791,7 @@
         <v>11</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E297" s="1" t="s">
         <v>12</v>
@@ -13808,7 +13808,7 @@
         <v>11</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E298" s="1" t="s">
         <v>12</v>
@@ -13825,7 +13825,7 @@
         <v>11</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E299" s="1" t="e">
         <v>#N/A</v>
@@ -13842,7 +13842,7 @@
         <v>11</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E300" s="1" t="s">
         <v>12</v>
@@ -13859,7 +13859,7 @@
         <v>11</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E301" s="1" t="s">
         <v>12</v>
@@ -13876,7 +13876,7 @@
         <v>11</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E302" s="1" t="s">
         <v>12</v>
@@ -13893,7 +13893,7 @@
         <v>11</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E303" s="1" t="s">
         <v>12</v>
@@ -13910,7 +13910,7 @@
         <v>11</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E304" s="1" t="s">
         <v>12</v>
@@ -13927,7 +13927,7 @@
         <v>11</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E305" s="1" t="s">
         <v>12</v>
@@ -13944,7 +13944,7 @@
         <v>11</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E306" s="1" t="s">
         <v>12</v>
@@ -13961,7 +13961,7 @@
         <v>11</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E307" s="1" t="s">
         <v>12</v>
@@ -13978,7 +13978,7 @@
         <v>11</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E308" s="1" t="s">
         <v>12</v>
@@ -13995,7 +13995,7 @@
         <v>11</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E309" s="1" t="s">
         <v>12</v>
@@ -14012,7 +14012,7 @@
         <v>11</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E310" s="1" t="s">
         <v>12</v>
@@ -14029,7 +14029,7 @@
         <v>11</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E311" s="1" t="s">
         <v>12</v>
@@ -14046,7 +14046,7 @@
         <v>11</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E312" s="1" t="s">
         <v>12</v>
@@ -14063,7 +14063,7 @@
         <v>11</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E313" s="1" t="s">
         <v>12</v>
@@ -14080,7 +14080,7 @@
         <v>11</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E314" s="1" t="s">
         <v>12</v>
@@ -14097,7 +14097,7 @@
         <v>11</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E315" s="1" t="s">
         <v>12</v>
@@ -14114,7 +14114,7 @@
         <v>11</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E316" s="1" t="s">
         <v>12</v>
@@ -14131,7 +14131,7 @@
         <v>11</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E317" s="1" t="s">
         <v>12</v>
@@ -14148,7 +14148,7 @@
         <v>11</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E318" s="1" t="s">
         <v>12</v>
@@ -14165,7 +14165,7 @@
         <v>11</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E319" s="1" t="s">
         <v>12</v>
@@ -14182,7 +14182,7 @@
         <v>11</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E320" s="1" t="s">
         <v>12</v>
@@ -14199,7 +14199,7 @@
         <v>11</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E321" s="1" t="s">
         <v>12</v>
@@ -14216,7 +14216,7 @@
         <v>11</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E322" s="1" t="s">
         <v>12</v>
@@ -14233,7 +14233,7 @@
         <v>11</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E323" s="1" t="s">
         <v>12</v>
@@ -14250,7 +14250,7 @@
         <v>11</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E324" s="1" t="s">
         <v>12</v>
@@ -14267,7 +14267,7 @@
         <v>11</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E325" s="1" t="s">
         <v>12</v>
@@ -14284,7 +14284,7 @@
         <v>11</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E326" s="1" t="s">
         <v>12</v>
@@ -14301,7 +14301,7 @@
         <v>11</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E327" s="1" t="s">
         <v>12</v>
@@ -14318,7 +14318,7 @@
         <v>11</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E328" s="1" t="s">
         <v>12</v>
@@ -14335,7 +14335,7 @@
         <v>11</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E329" s="1" t="s">
         <v>12</v>
@@ -14352,7 +14352,7 @@
         <v>11</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E330" s="1" t="s">
         <v>12</v>
@@ -14369,7 +14369,7 @@
         <v>11</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E331" s="1" t="s">
         <v>12</v>
@@ -14386,7 +14386,7 @@
         <v>11</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E332" s="1" t="s">
         <v>12</v>
@@ -14403,7 +14403,7 @@
         <v>11</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E333" s="1" t="s">
         <v>12</v>
@@ -14420,7 +14420,7 @@
         <v>11</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E334" s="1" t="s">
         <v>12</v>
@@ -14437,7 +14437,7 @@
         <v>11</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E335" s="1" t="s">
         <v>12</v>
@@ -14454,7 +14454,7 @@
         <v>11</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E336" s="1" t="s">
         <v>12</v>
@@ -14471,7 +14471,7 @@
         <v>11</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E337" s="1" t="s">
         <v>12</v>
@@ -14488,7 +14488,7 @@
         <v>11</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E338" s="1" t="s">
         <v>12</v>
@@ -14505,7 +14505,7 @@
         <v>11</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E339" s="1" t="s">
         <v>12</v>
@@ -14522,7 +14522,7 @@
         <v>11</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E340" s="1" t="s">
         <v>12</v>
@@ -14539,7 +14539,7 @@
         <v>11</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E341" s="1" t="s">
         <v>12</v>
@@ -14556,7 +14556,7 @@
         <v>11</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E342" s="1" t="s">
         <v>12</v>
@@ -14573,7 +14573,7 @@
         <v>11</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E343" s="1" t="s">
         <v>12</v>
@@ -14590,7 +14590,7 @@
         <v>11</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>12</v>
@@ -14607,7 +14607,7 @@
         <v>11</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E345" s="1" t="s">
         <v>12</v>
@@ -14624,7 +14624,7 @@
         <v>11</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E346" s="1" t="s">
         <v>12</v>
@@ -14641,7 +14641,7 @@
         <v>11</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E347" s="1" t="s">
         <v>12</v>
@@ -14658,7 +14658,7 @@
         <v>11</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E348" s="1" t="s">
         <v>12</v>
@@ -14675,7 +14675,7 @@
         <v>11</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E349" s="1" t="s">
         <v>12</v>
@@ -14692,7 +14692,7 @@
         <v>11</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E350" s="1" t="s">
         <v>12</v>
@@ -14709,7 +14709,7 @@
         <v>11</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E351" s="1" t="s">
         <v>12</v>
@@ -14726,7 +14726,7 @@
         <v>11</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E352" s="1" t="s">
         <v>12</v>
@@ -14743,7 +14743,7 @@
         <v>11</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E353" s="1" t="s">
         <v>12</v>
@@ -14760,7 +14760,7 @@
         <v>11</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E354" s="1" t="s">
         <v>12</v>
@@ -14777,7 +14777,7 @@
         <v>11</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E355" s="1" t="s">
         <v>12</v>
@@ -14794,7 +14794,7 @@
         <v>11</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E356" s="1" t="s">
         <v>12</v>
@@ -14811,7 +14811,7 @@
         <v>11</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E357" s="1" t="s">
         <v>12</v>
@@ -14828,7 +14828,7 @@
         <v>11</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E358" s="1" t="s">
         <v>12</v>
@@ -14845,7 +14845,7 @@
         <v>11</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E359" s="1" t="s">
         <v>12</v>
@@ -14862,7 +14862,7 @@
         <v>11</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E360" s="1" t="s">
         <v>12</v>
@@ -14879,7 +14879,7 @@
         <v>11</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E361" s="1" t="s">
         <v>12</v>
@@ -14896,7 +14896,7 @@
         <v>11</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E362" s="1" t="s">
         <v>12</v>
@@ -14913,7 +14913,7 @@
         <v>11</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E363" s="1" t="s">
         <v>12</v>
@@ -14930,7 +14930,7 @@
         <v>11</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E364" s="1" t="s">
         <v>12</v>
@@ -14947,7 +14947,7 @@
         <v>11</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E365" s="1" t="s">
         <v>12</v>
@@ -14964,7 +14964,7 @@
         <v>11</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E366" s="1" t="s">
         <v>12</v>
@@ -14981,7 +14981,7 @@
         <v>11</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E367" s="1" t="s">
         <v>12</v>
@@ -14998,7 +14998,7 @@
         <v>11</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E368" s="1" t="s">
         <v>12</v>
@@ -15015,7 +15015,7 @@
         <v>11</v>
       </c>
       <c r="D369" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E369" s="1" t="s">
         <v>12</v>
@@ -15032,7 +15032,7 @@
         <v>11</v>
       </c>
       <c r="D370" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E370" s="1" t="s">
         <v>12</v>
@@ -15049,7 +15049,7 @@
         <v>11</v>
       </c>
       <c r="D371" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E371" s="1" t="s">
         <v>12</v>
@@ -15066,7 +15066,7 @@
         <v>11</v>
       </c>
       <c r="D372" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E372" s="1" t="s">
         <v>12</v>
@@ -15083,7 +15083,7 @@
         <v>11</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E373" s="1" t="s">
         <v>12</v>
@@ -15100,7 +15100,7 @@
         <v>11</v>
       </c>
       <c r="D374" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E374" s="1" t="s">
         <v>12</v>
@@ -15117,7 +15117,7 @@
         <v>11</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E375" s="1" t="s">
         <v>12</v>
@@ -15134,7 +15134,7 @@
         <v>11</v>
       </c>
       <c r="D376" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E376" s="1" t="s">
         <v>12</v>
@@ -15151,7 +15151,7 @@
         <v>11</v>
       </c>
       <c r="D377" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E377" s="1" t="s">
         <v>12</v>
@@ -15168,7 +15168,7 @@
         <v>11</v>
       </c>
       <c r="D378" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E378" s="1" t="s">
         <v>12</v>
@@ -15185,7 +15185,7 @@
         <v>11</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E379" s="1" t="s">
         <v>12</v>
@@ -15202,7 +15202,7 @@
         <v>11</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E380" s="1" t="s">
         <v>12</v>
@@ -15219,7 +15219,7 @@
         <v>11</v>
       </c>
       <c r="D381" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E381" s="1" t="s">
         <v>12</v>
@@ -15236,7 +15236,7 @@
         <v>11</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E382" s="1" t="s">
         <v>12</v>
@@ -15253,7 +15253,7 @@
         <v>11</v>
       </c>
       <c r="D383" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E383" s="1" t="s">
         <v>12</v>
@@ -15270,7 +15270,7 @@
         <v>11</v>
       </c>
       <c r="D384" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E384" s="1" t="s">
         <v>12</v>
@@ -15287,7 +15287,7 @@
         <v>11</v>
       </c>
       <c r="D385" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E385" s="1" t="s">
         <v>12</v>
@@ -15304,7 +15304,7 @@
         <v>11</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E386" s="1" t="s">
         <v>12</v>
@@ -15321,7 +15321,7 @@
         <v>11</v>
       </c>
       <c r="D387" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E387" s="1" t="s">
         <v>12</v>
@@ -15338,7 +15338,7 @@
         <v>11</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E388" s="1" t="s">
         <v>12</v>
@@ -15355,7 +15355,7 @@
         <v>11</v>
       </c>
       <c r="D389" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E389" s="1" t="s">
         <v>12</v>
@@ -15372,7 +15372,7 @@
         <v>11</v>
       </c>
       <c r="D390" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E390" s="1" t="s">
         <v>12</v>
@@ -15389,7 +15389,7 @@
         <v>11</v>
       </c>
       <c r="D391" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E391" s="1" t="s">
         <v>12</v>
@@ -15406,7 +15406,7 @@
         <v>11</v>
       </c>
       <c r="D392" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E392" s="1" t="s">
         <v>12</v>
@@ -15423,7 +15423,7 @@
         <v>11</v>
       </c>
       <c r="D393" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E393" s="1" t="s">
         <v>12</v>
@@ -15440,7 +15440,7 @@
         <v>11</v>
       </c>
       <c r="D394" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E394" s="1" t="s">
         <v>12</v>
@@ -15457,7 +15457,7 @@
         <v>11</v>
       </c>
       <c r="D395" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E395" s="1" t="s">
         <v>12</v>
@@ -15474,7 +15474,7 @@
         <v>11</v>
       </c>
       <c r="D396" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E396" s="1" t="s">
         <v>12</v>
@@ -15491,7 +15491,7 @@
         <v>11</v>
       </c>
       <c r="D397" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E397" s="1" t="s">
         <v>12</v>
@@ -15508,7 +15508,7 @@
         <v>11</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E398" s="1" t="s">
         <v>12</v>
@@ -15525,7 +15525,7 @@
         <v>11</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E399" s="1" t="s">
         <v>12</v>
@@ -15542,7 +15542,7 @@
         <v>11</v>
       </c>
       <c r="D400" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E400" s="1" t="s">
         <v>12</v>
@@ -15559,7 +15559,7 @@
         <v>11</v>
       </c>
       <c r="D401" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E401" s="1" t="s">
         <v>12</v>
@@ -15576,7 +15576,7 @@
         <v>11</v>
       </c>
       <c r="D402" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E402" s="1" t="s">
         <v>12</v>
@@ -15593,7 +15593,7 @@
         <v>11</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E403" s="1" t="s">
         <v>12</v>
@@ -15610,7 +15610,7 @@
         <v>11</v>
       </c>
       <c r="D404" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E404" s="1" t="s">
         <v>12</v>
@@ -15627,7 +15627,7 @@
         <v>11</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E405" s="1" t="s">
         <v>12</v>
@@ -15644,7 +15644,7 @@
         <v>11</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E406" s="1" t="s">
         <v>12</v>
@@ -15661,7 +15661,7 @@
         <v>11</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E407" s="1" t="s">
         <v>12</v>
@@ -15678,7 +15678,7 @@
         <v>11</v>
       </c>
       <c r="D408" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E408" s="1" t="s">
         <v>12</v>
@@ -15695,7 +15695,7 @@
         <v>11</v>
       </c>
       <c r="D409" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E409" s="1" t="s">
         <v>12</v>
@@ -15712,7 +15712,7 @@
         <v>11</v>
       </c>
       <c r="D410" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E410" s="1" t="s">
         <v>12</v>
@@ -15729,7 +15729,7 @@
         <v>11</v>
       </c>
       <c r="D411" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E411" s="1" t="s">
         <v>12</v>
@@ -15746,7 +15746,7 @@
         <v>11</v>
       </c>
       <c r="D412" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E412" s="1" t="s">
         <v>12</v>
@@ -15763,7 +15763,7 @@
         <v>11</v>
       </c>
       <c r="D413" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E413" s="1" t="s">
         <v>12</v>
@@ -15780,7 +15780,7 @@
         <v>11</v>
       </c>
       <c r="D414" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E414" s="1" t="s">
         <v>12</v>
@@ -15797,7 +15797,7 @@
         <v>11</v>
       </c>
       <c r="D415" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E415" s="1" t="s">
         <v>12</v>
@@ -15814,7 +15814,7 @@
         <v>11</v>
       </c>
       <c r="D416" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E416" s="1" t="e">
         <v>#N/A</v>
@@ -15831,7 +15831,7 @@
         <v>11</v>
       </c>
       <c r="D417" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E417" s="1" t="s">
         <v>12</v>
@@ -15848,7 +15848,7 @@
         <v>11</v>
       </c>
       <c r="D418" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E418" s="1" t="s">
         <v>12</v>
@@ -15865,7 +15865,7 @@
         <v>11</v>
       </c>
       <c r="D419" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E419" s="1" t="e">
         <v>#N/A</v>
@@ -15882,7 +15882,7 @@
         <v>11</v>
       </c>
       <c r="D420" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E420" s="1" t="s">
         <v>12</v>
@@ -15899,7 +15899,7 @@
         <v>11</v>
       </c>
       <c r="D421" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E421" s="1" t="s">
         <v>12</v>
@@ -15916,7 +15916,7 @@
         <v>11</v>
       </c>
       <c r="D422" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E422" s="1" t="s">
         <v>12</v>
@@ -15933,7 +15933,7 @@
         <v>11</v>
       </c>
       <c r="D423" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E423" s="1" t="s">
         <v>12</v>
@@ -15950,7 +15950,7 @@
         <v>11</v>
       </c>
       <c r="D424" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E424" s="1" t="s">
         <v>12</v>
@@ -15967,7 +15967,7 @@
         <v>11</v>
       </c>
       <c r="D425" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E425" s="1" t="s">
         <v>12</v>
@@ -15984,7 +15984,7 @@
         <v>11</v>
       </c>
       <c r="D426" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E426" s="1" t="s">
         <v>12</v>
@@ -16001,7 +16001,7 @@
         <v>11</v>
       </c>
       <c r="D427" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E427" s="1" t="s">
         <v>12</v>
@@ -16018,7 +16018,7 @@
         <v>11</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E428" s="1" t="s">
         <v>12</v>
@@ -16035,7 +16035,7 @@
         <v>11</v>
       </c>
       <c r="D429" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E429" s="1" t="s">
         <v>12</v>
@@ -16052,7 +16052,7 @@
         <v>11</v>
       </c>
       <c r="D430" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E430" s="1" t="s">
         <v>12</v>
@@ -16069,7 +16069,7 @@
         <v>11</v>
       </c>
       <c r="D431" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E431" s="1" t="s">
         <v>12</v>
@@ -16086,7 +16086,7 @@
         <v>11</v>
       </c>
       <c r="D432" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E432" s="1" t="s">
         <v>12</v>
@@ -16103,7 +16103,7 @@
         <v>11</v>
       </c>
       <c r="D433" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E433" s="1" t="s">
         <v>12</v>
@@ -16120,7 +16120,7 @@
         <v>11</v>
       </c>
       <c r="D434" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E434" s="1" t="s">
         <v>12</v>
@@ -16137,7 +16137,7 @@
         <v>11</v>
       </c>
       <c r="D435" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E435" s="1" t="s">
         <v>12</v>
@@ -16154,7 +16154,7 @@
         <v>11</v>
       </c>
       <c r="D436" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E436" s="1" t="e">
         <v>#N/A</v>
@@ -16171,7 +16171,7 @@
         <v>11</v>
       </c>
       <c r="D437" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E437" s="1" t="s">
         <v>12</v>
@@ -16188,7 +16188,7 @@
         <v>11</v>
       </c>
       <c r="D438" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E438" s="1" t="s">
         <v>12</v>
@@ -16205,7 +16205,7 @@
         <v>11</v>
       </c>
       <c r="D439" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E439" s="1" t="s">
         <v>12</v>
@@ -16222,7 +16222,7 @@
         <v>11</v>
       </c>
       <c r="D440" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E440" s="1" t="s">
         <v>12</v>
@@ -16239,7 +16239,7 @@
         <v>11</v>
       </c>
       <c r="D441" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E441" s="1" t="e">
         <v>#N/A</v>
@@ -16256,7 +16256,7 @@
         <v>11</v>
       </c>
       <c r="D442" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E442" s="1" t="e">
         <v>#N/A</v>
@@ -16273,7 +16273,7 @@
         <v>11</v>
       </c>
       <c r="D443" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E443" s="1" t="e">
         <v>#N/A</v>
@@ -16290,7 +16290,7 @@
         <v>11</v>
       </c>
       <c r="D444" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E444" s="1" t="e">
         <v>#N/A</v>
@@ -16307,7 +16307,7 @@
         <v>11</v>
       </c>
       <c r="D445" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E445" s="1" t="e">
         <v>#N/A</v>
@@ -16324,7 +16324,7 @@
         <v>11</v>
       </c>
       <c r="D446" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E446" s="1" t="e">
         <v>#N/A</v>
@@ -16341,7 +16341,7 @@
         <v>11</v>
       </c>
       <c r="D447" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E447" s="1" t="e">
         <v>#N/A</v>
@@ -16358,7 +16358,7 @@
         <v>11</v>
       </c>
       <c r="D448" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E448" s="1" t="s">
         <v>12</v>
@@ -16375,7 +16375,7 @@
         <v>11</v>
       </c>
       <c r="D449" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E449" s="1" t="e">
         <v>#N/A</v>
@@ -16392,7 +16392,7 @@
         <v>11</v>
       </c>
       <c r="D450" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E450" s="1" t="e">
         <v>#N/A</v>
@@ -16409,7 +16409,7 @@
         <v>11</v>
       </c>
       <c r="D451" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E451" s="1" t="e">
         <v>#N/A</v>
@@ -16426,7 +16426,7 @@
         <v>11</v>
       </c>
       <c r="D452" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E452" s="1" t="e">
         <v>#N/A</v>
@@ -16443,7 +16443,7 @@
         <v>11</v>
       </c>
       <c r="D453" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E453" s="1" t="e">
         <v>#N/A</v>
@@ -16460,7 +16460,7 @@
         <v>11</v>
       </c>
       <c r="D454" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E454" s="1" t="e">
         <v>#N/A</v>
@@ -16477,7 +16477,7 @@
         <v>11</v>
       </c>
       <c r="D455" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E455" s="1" t="e">
         <v>#N/A</v>
@@ -16494,7 +16494,7 @@
         <v>11</v>
       </c>
       <c r="D456" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E456" s="1" t="e">
         <v>#N/A</v>
@@ -16511,7 +16511,7 @@
         <v>11</v>
       </c>
       <c r="D457" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E457" s="1" t="e">
         <v>#N/A</v>
@@ -16528,7 +16528,7 @@
         <v>11</v>
       </c>
       <c r="D458" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E458" s="1" t="e">
         <v>#N/A</v>
@@ -16545,7 +16545,7 @@
         <v>11</v>
       </c>
       <c r="D459" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E459" s="1" t="s">
         <v>12</v>

</xml_diff>